<commit_message>
Thêm search đã học
</commit_message>
<xml_diff>
--- a/src/data/dataFile/xlsx/oldWord/oldWord.xlsx
+++ b/src/data/dataFile/xlsx/oldWord/oldWord.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>English</t>
   </si>
@@ -24,30 +24,6 @@
   </si>
   <si>
     <t>PathImage</t>
-  </si>
-  <si>
-    <t>pink</t>
-  </si>
-  <si>
-    <t>màu hồng</t>
-  </si>
-  <si>
-    <t>easy</t>
-  </si>
-  <si>
-    <t>src\data\dataFile\img\color\pink.png</t>
-  </si>
-  <si>
-    <t>white</t>
-  </si>
-  <si>
-    <t>màu trắng</t>
-  </si>
-  <si>
-    <t>moderate</t>
-  </si>
-  <si>
-    <t>src\data\dataFile\img\color\white.JPG</t>
   </si>
 </sst>
 </file>
@@ -112,34 +88,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>